<commit_message>
[woo] action_group_player에 버튼 출력 텍스트 추가
</commit_message>
<xml_diff>
--- a/Assets/Resource/ExcelData/action_group_player.xlsx
+++ b/Assets/Resource/ExcelData/action_group_player.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\TextRPG\Assets\Resource\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC486661-3734-4596-AA61-4EE5905031FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BD80FA-FBD5-41AF-8320-97E747D030A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6096" yWindow="5772" windowWidth="35832" windowHeight="19692" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
+    <workbookView xWindow="5928" yWindow="17340" windowWidth="35832" windowHeight="19692" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
   <sheets>
     <sheet name="action_group_player" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>string</t>
   </si>
@@ -96,6 +96,34 @@
   </si>
   <si>
     <t>텍스트 우선순위 높음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>button_text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버튼 텍스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빈틈 노리기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격 회피하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저지하기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -520,143 +548,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9A91B-D08A-4539-AB73-212820098BCC}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="12" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.796875" style="3"/>
+    <col min="2" max="3" width="40" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="5" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="5" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="b">
+      <c r="D4" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="b">
+      <c r="D5" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1" t="b">
+      <c r="D6" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="b">
+      <c r="D7" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -665,8 +725,9 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -675,8 +736,9 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -685,6 +747,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>